<commit_message>
Updated Traceability Matrix with Use Case specification document names.
</commit_message>
<xml_diff>
--- a/Ice Cream Manager/Documentation/Working Documents/Traceability Matrix.xlsx
+++ b/Ice Cream Manager/Documentation/Working Documents/Traceability Matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>SPMP</t>
   </si>
@@ -45,6 +45,72 @@
   </si>
   <si>
     <t>UCSD</t>
+  </si>
+  <si>
+    <t>UC01</t>
+  </si>
+  <si>
+    <t>UC02</t>
+  </si>
+  <si>
+    <t>UC03</t>
+  </si>
+  <si>
+    <t>UC04</t>
+  </si>
+  <si>
+    <t>UC05</t>
+  </si>
+  <si>
+    <t>UC06</t>
+  </si>
+  <si>
+    <t>UC07</t>
+  </si>
+  <si>
+    <t>UC08</t>
+  </si>
+  <si>
+    <t>UC09</t>
+  </si>
+  <si>
+    <t>UC10</t>
+  </si>
+  <si>
+    <t>UC11</t>
+  </si>
+  <si>
+    <t>Use Case - Modify Item</t>
+  </si>
+  <si>
+    <t>Use Case - Modify Inventory</t>
+  </si>
+  <si>
+    <t>Use Case - View Sales</t>
+  </si>
+  <si>
+    <t>Use Case - Modify Route</t>
+  </si>
+  <si>
+    <t>Use Case - Modify Truck</t>
+  </si>
+  <si>
+    <t>Use Case - Process Batch File</t>
+  </si>
+  <si>
+    <t>Use Case - Modify Driver</t>
+  </si>
+  <si>
+    <t>Use Case - Modify Settings</t>
+  </si>
+  <si>
+    <t>Use Case - Modify Voting</t>
+  </si>
+  <si>
+    <t>Use Case - Modify Presets</t>
+  </si>
+  <si>
+    <t>Use Case - View Fuel Usage</t>
   </si>
 </sst>
 </file>
@@ -434,7 +500,7 @@
   <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -462,49 +528,49 @@
         <f>B4</f>
         <v>UCSD</v>
       </c>
-      <c r="F1" s="5">
+      <c r="F1" s="5" t="str">
         <f>B5</f>
-        <v>0</v>
-      </c>
-      <c r="G1" s="5">
+        <v>UC01</v>
+      </c>
+      <c r="G1" s="5" t="str">
         <f>B6</f>
-        <v>0</v>
-      </c>
-      <c r="H1" s="5">
+        <v>UC02</v>
+      </c>
+      <c r="H1" s="5" t="str">
         <f>B7</f>
-        <v>0</v>
-      </c>
-      <c r="I1" s="5">
+        <v>UC03</v>
+      </c>
+      <c r="I1" s="5" t="str">
         <f>B8</f>
-        <v>0</v>
-      </c>
-      <c r="J1" s="5">
+        <v>UC04</v>
+      </c>
+      <c r="J1" s="5" t="str">
         <f>B9</f>
-        <v>0</v>
-      </c>
-      <c r="K1" s="5">
+        <v>UC05</v>
+      </c>
+      <c r="K1" s="5" t="str">
         <f>B10</f>
-        <v>0</v>
-      </c>
-      <c r="L1" s="5">
+        <v>UC06</v>
+      </c>
+      <c r="L1" s="5" t="str">
         <f>B11</f>
-        <v>0</v>
-      </c>
-      <c r="M1" s="5">
+        <v>UC07</v>
+      </c>
+      <c r="M1" s="5" t="str">
         <f>B12</f>
-        <v>0</v>
-      </c>
-      <c r="N1" s="5">
+        <v>UC08</v>
+      </c>
+      <c r="N1" s="5" t="str">
         <f>B13</f>
-        <v>0</v>
-      </c>
-      <c r="O1" s="5">
+        <v>UC09</v>
+      </c>
+      <c r="O1" s="5" t="str">
         <f>B14</f>
-        <v>0</v>
-      </c>
-      <c r="P1" s="5">
+        <v>UC10</v>
+      </c>
+      <c r="P1" s="5" t="str">
         <f>B15</f>
-        <v>0</v>
+        <v>UC11</v>
       </c>
       <c r="Q1" s="5">
         <f>B16</f>
@@ -524,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="9"/>
-      <c r="D2" s="7"/>
+      <c r="D2" s="9"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -547,7 +613,7 @@
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="7"/>
@@ -589,8 +655,12 @@
       <c r="R4" s="7"/>
     </row>
     <row r="5" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="8"/>
+      <c r="A5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -609,8 +679,12 @@
       <c r="R5" s="7"/>
     </row>
     <row r="6" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -629,8 +703,12 @@
       <c r="R6" s="7"/>
     </row>
     <row r="7" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="8"/>
+      <c r="A7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -649,8 +727,12 @@
       <c r="R7" s="7"/>
     </row>
     <row r="8" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -669,8 +751,12 @@
       <c r="R8" s="7"/>
     </row>
     <row r="9" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
+      <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -689,8 +775,12 @@
       <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -709,8 +799,12 @@
       <c r="R10" s="7"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -729,8 +823,12 @@
       <c r="R11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -749,8 +847,12 @@
       <c r="R12" s="7"/>
     </row>
     <row r="13" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -769,8 +871,12 @@
       <c r="R13" s="7"/>
     </row>
     <row r="14" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -789,8 +895,12 @@
       <c r="R14" s="7"/>
     </row>
     <row r="15" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="8"/>
+      <c r="A15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>

</xml_diff>

<commit_message>
Added relationships between UC05 and any use case that can be performed by the Process actor; UC01, UC03, UC04, UC06, UC07.
</commit_message>
<xml_diff>
--- a/Ice Cream Manager/Documentation/Working Documents/Traceability Matrix.xlsx
+++ b/Ice Cream Manager/Documentation/Working Documents/Traceability Matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marck\Documents\GitHubVisualStudio\cosmosys\Ice Cream Manager\Documentation\Working Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cosmosys\Ice Cream Manager\Documentation\Working Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -117,7 +117,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,8 +136,13 @@
       <color theme="1"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +152,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -200,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -217,6 +228,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,7 +513,7 @@
   <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -640,17 +653,17 @@
       <c r="C4" s="7"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
     </row>
@@ -663,12 +676,12 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="9"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="J5" s="9"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -687,7 +700,7 @@
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="9"/>
       <c r="H6" s="7"/>
@@ -711,12 +724,12 @@
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="10"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="9"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="9"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
@@ -735,12 +748,12 @@
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="7"/>
+      <c r="J8" s="9"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
@@ -759,14 +772,14 @@
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="9"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
@@ -783,12 +796,12 @@
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
@@ -807,12 +820,12 @@
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+      <c r="J11" s="9"/>
       <c r="K11" s="7"/>
       <c r="L11" s="9"/>
       <c r="M11" s="7"/>
@@ -831,7 +844,7 @@
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="10"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -855,7 +868,7 @@
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -879,7 +892,7 @@
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -903,7 +916,7 @@
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>

</xml_diff>